<commit_message>
Add USs related to cluster domain "Social and Urban Studies" [Transportations]
</commit_message>
<xml_diff>
--- a/refair-server/datasets/FSDataset-2.xlsx
+++ b/refair-server/datasets/FSDataset-2.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="806" uniqueCount="197">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="906" uniqueCount="218">
   <si>
     <t>Domain Cluster</t>
   </si>
@@ -602,6 +602,69 @@
   </si>
   <si>
     <t>As a social scientist, I want to use word embedding algorithms to analyze student essays discussing cultural diversity to identify underlying themes and perspectives on multiculturalism in educational settings.</t>
+  </si>
+  <si>
+    <t>Transportations</t>
+  </si>
+  <si>
+    <t>As a logistics manager, I want to employ adversarial learning models to identify fraudulent activities in shipment tracking systems, so that I can prevent cargo theft and ensure the integrity of supply chain operations.</t>
+  </si>
+  <si>
+    <t>As a railway operator, I want to employ CNN architectures to analyze track condition images captured by drones, so that I can detect defects early, schedule maintenance proactively, and improve overall safety and reliability.</t>
+  </si>
+  <si>
+    <t>As an airport information desk operator, I want to implement a conversational agent to help travelers navigate through the airport, find amenities, and receive real-time updates on flight statuses, so that I can enhance customer satisfaction and streamline operations.</t>
+  </si>
+  <si>
+    <t>As a traffic engineer, I want to use decision tree models to analyze historical traffic data and identify key factors contributing to congestion at specific intersections, so that I can optimize traffic signal timings and improve traffic flow.</t>
+  </si>
+  <si>
+    <t>As a safety compliance officer for a transportation company, I want to implement document classification models to categorize and prioritize incident reports and safety inspection records, so that I can identify trends, assess risks, and improve safety protocols.</t>
+  </si>
+  <si>
+    <t>As an airline operations manager, I want to deploy entity extraction models to automatically extract flight details including departure times, arrival times, flight numbers, and destinations from flight schedules and booking confirmations, so that I can monitor flight statuses and manage operations more effectively.</t>
+  </si>
+  <si>
+    <t>As a logistics planner, I want to use feature selection techniques to identify key variables in shipment data that impact delivery times, such as distance, mode of transport, and traffic conditions, so that I can improve delivery efficiency and customer satisfaction.</t>
+  </si>
+  <si>
+    <t>As a railway safety officer, I want to address the imbalanced dataset in incident reports to improve the accuracy of predicting rare but critical safety incidents, such as derailments or collisions, so that I can implement targeted safety measures and reduce risks.</t>
+  </si>
+  <si>
+    <t>As a public transport planner, I want to utilize k-NN algorithms to recommend optimal transit routes to commuters based on their historical travel patterns and current traffic conditions, so that I can enhance commuter satisfaction and promote the use of public transportation.</t>
+  </si>
+  <si>
+    <t>As a transportation planner, I want to apply keyword extraction methods to analyze public feedback and comments on transportation services to identify key concerns and suggestions, so that I can improve service quality and customer satisfaction.</t>
+  </si>
+  <si>
+    <t>As a cargo logistics manager, I want to use multi-label classification to predict the types of goods being transported based on shipment descriptions, so that I can ensure proper handling, storage, and compliance with transport regulations.</t>
+  </si>
+  <si>
+    <t>As an autonomous vehicle developer, I want to train neural networks to recognize and classify different types of road obstacles and hazards from sensor data, such as pedestrians, cyclists, and road debris, so that I can improve the vehicle's ability to navigate safely.</t>
+  </si>
+  <si>
+    <t>As a logistics manager, I want to deploy a random forest algorithm to classify delivery routes based on factors such as distance, road conditions, and delivery time windows, so that I can optimize route planning and ensure timely deliveries.</t>
+  </si>
+  <si>
+    <t>As a traffic management system developer, I want to implement semantic similarity algorithms to identify similar traffic incident reports and prioritize response efforts based on the severity and impact on traffic flow, so that I can improve incident management efficiency.</t>
+  </si>
+  <si>
+    <t>As a public transport planner, I want to use sentiment analysis to analyze commuter sentiment towards different routes and services based on social media posts and surveys, so that I can prioritize enhancements and adjustments in public transport offerings.</t>
+  </si>
+  <si>
+    <t>As a railway station announcer, I want to deploy speech-to-text systems to transcribe train arrival and departure announcements in real-time, so that I can provide accurate and timely information to passengers, especially in noisy or crowded environments.</t>
+  </si>
+  <si>
+    <t>As an airport operations manager, I want to utilize text categorization algorithms to categorize passenger feedback received through surveys and comment cards into categories such as facilities, staff interactions, and amenities, so that I can identify areas for improvement and enhance passenger experience.</t>
+  </si>
+  <si>
+    <t>As a traffic management engineer, I want to use unsupervised clustering algorithms to group traffic sensors based on similar traffic patterns and congestion levels, so that I can identify critical areas for traffic flow optimization and signal timing adjustments.</t>
+  </si>
+  <si>
+    <t>As a railway station announcer, I want to deploy voice recognition software to automatically transcribe and broadcast train departure and arrival announcements, so that I can ensure accurate and timely information for passengers.</t>
+  </si>
+  <si>
+    <t>As a logistics planner, I want to use word embedding models to analyze customer feedback and identify key themes and sentiments related to delivery services, so that I can prioritize improvements and enhance customer satisfaction.</t>
   </si>
 </sst>
 </file>
@@ -659,7 +722,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -718,6 +781,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FF783F04"/>
         <bgColor rgb="FF783F04"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF990000"/>
+        <bgColor rgb="FF990000"/>
       </patternFill>
     </fill>
   </fills>
@@ -797,7 +866,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="43">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -916,6 +985,15 @@
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="11" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="11" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" vertical="top"/>
+    </xf>
+    <xf borderId="0" fillId="11" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
@@ -4361,6 +4439,406 @@
         <v>10</v>
       </c>
     </row>
+    <row r="162">
+      <c r="A162" s="40" t="s">
+        <v>70</v>
+      </c>
+      <c r="B162" s="41">
+        <v>7.0</v>
+      </c>
+      <c r="C162" s="42" t="s">
+        <v>197</v>
+      </c>
+      <c r="D162" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="E162" s="39" t="s">
+        <v>198</v>
+      </c>
+      <c r="F162" s="8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="163">
+      <c r="A163" s="40" t="s">
+        <v>70</v>
+      </c>
+      <c r="B163" s="41">
+        <v>7.0</v>
+      </c>
+      <c r="C163" s="42" t="s">
+        <v>197</v>
+      </c>
+      <c r="D163" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="E163" s="39" t="s">
+        <v>199</v>
+      </c>
+      <c r="F163" s="8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="164">
+      <c r="A164" s="40" t="s">
+        <v>70</v>
+      </c>
+      <c r="B164" s="41">
+        <v>7.0</v>
+      </c>
+      <c r="C164" s="42" t="s">
+        <v>197</v>
+      </c>
+      <c r="D164" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="E164" s="39" t="s">
+        <v>200</v>
+      </c>
+      <c r="F164" s="8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="165">
+      <c r="A165" s="40" t="s">
+        <v>70</v>
+      </c>
+      <c r="B165" s="41">
+        <v>7.0</v>
+      </c>
+      <c r="C165" s="42" t="s">
+        <v>197</v>
+      </c>
+      <c r="D165" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="E165" s="39" t="s">
+        <v>201</v>
+      </c>
+      <c r="F165" s="8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="166">
+      <c r="A166" s="40" t="s">
+        <v>70</v>
+      </c>
+      <c r="B166" s="41">
+        <v>7.0</v>
+      </c>
+      <c r="C166" s="42" t="s">
+        <v>197</v>
+      </c>
+      <c r="D166" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="E166" s="39" t="s">
+        <v>202</v>
+      </c>
+      <c r="F166" s="8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="167">
+      <c r="A167" s="40" t="s">
+        <v>70</v>
+      </c>
+      <c r="B167" s="41">
+        <v>7.0</v>
+      </c>
+      <c r="C167" s="42" t="s">
+        <v>197</v>
+      </c>
+      <c r="D167" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="E167" s="39" t="s">
+        <v>203</v>
+      </c>
+      <c r="F167" s="8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="168">
+      <c r="A168" s="40" t="s">
+        <v>70</v>
+      </c>
+      <c r="B168" s="41">
+        <v>7.0</v>
+      </c>
+      <c r="C168" s="42" t="s">
+        <v>197</v>
+      </c>
+      <c r="D168" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="E168" s="39" t="s">
+        <v>204</v>
+      </c>
+      <c r="F168" s="8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="169">
+      <c r="A169" s="40" t="s">
+        <v>70</v>
+      </c>
+      <c r="B169" s="41">
+        <v>7.0</v>
+      </c>
+      <c r="C169" s="42" t="s">
+        <v>197</v>
+      </c>
+      <c r="D169" s="21" t="s">
+        <v>31</v>
+      </c>
+      <c r="E169" s="39" t="s">
+        <v>205</v>
+      </c>
+      <c r="F169" s="8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="170">
+      <c r="A170" s="40" t="s">
+        <v>70</v>
+      </c>
+      <c r="B170" s="41">
+        <v>7.0</v>
+      </c>
+      <c r="C170" s="42" t="s">
+        <v>197</v>
+      </c>
+      <c r="D170" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="E170" s="39" t="s">
+        <v>206</v>
+      </c>
+      <c r="F170" s="8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="171">
+      <c r="A171" s="40" t="s">
+        <v>70</v>
+      </c>
+      <c r="B171" s="41">
+        <v>7.0</v>
+      </c>
+      <c r="C171" s="42" t="s">
+        <v>197</v>
+      </c>
+      <c r="D171" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="E171" s="39" t="s">
+        <v>207</v>
+      </c>
+      <c r="F171" s="8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="172">
+      <c r="A172" s="40" t="s">
+        <v>70</v>
+      </c>
+      <c r="B172" s="41">
+        <v>7.0</v>
+      </c>
+      <c r="C172" s="42" t="s">
+        <v>197</v>
+      </c>
+      <c r="D172" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="E172" s="39" t="s">
+        <v>208</v>
+      </c>
+      <c r="F172" s="8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="173">
+      <c r="A173" s="40" t="s">
+        <v>70</v>
+      </c>
+      <c r="B173" s="41">
+        <v>7.0</v>
+      </c>
+      <c r="C173" s="42" t="s">
+        <v>197</v>
+      </c>
+      <c r="D173" s="21" t="s">
+        <v>43</v>
+      </c>
+      <c r="E173" s="39" t="s">
+        <v>209</v>
+      </c>
+      <c r="F173" s="8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="174">
+      <c r="A174" s="40" t="s">
+        <v>70</v>
+      </c>
+      <c r="B174" s="41">
+        <v>7.0</v>
+      </c>
+      <c r="C174" s="42" t="s">
+        <v>197</v>
+      </c>
+      <c r="D174" s="21" t="s">
+        <v>46</v>
+      </c>
+      <c r="E174" s="39" t="s">
+        <v>210</v>
+      </c>
+      <c r="F174" s="8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="175">
+      <c r="A175" s="40" t="s">
+        <v>70</v>
+      </c>
+      <c r="B175" s="41">
+        <v>7.0</v>
+      </c>
+      <c r="C175" s="42" t="s">
+        <v>197</v>
+      </c>
+      <c r="D175" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="E175" s="39" t="s">
+        <v>211</v>
+      </c>
+      <c r="F175" s="8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="176">
+      <c r="A176" s="40" t="s">
+        <v>70</v>
+      </c>
+      <c r="B176" s="41">
+        <v>7.0</v>
+      </c>
+      <c r="C176" s="42" t="s">
+        <v>197</v>
+      </c>
+      <c r="D176" s="21" t="s">
+        <v>52</v>
+      </c>
+      <c r="E176" s="39" t="s">
+        <v>212</v>
+      </c>
+      <c r="F176" s="8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="177">
+      <c r="A177" s="40" t="s">
+        <v>70</v>
+      </c>
+      <c r="B177" s="41">
+        <v>7.0</v>
+      </c>
+      <c r="C177" s="42" t="s">
+        <v>197</v>
+      </c>
+      <c r="D177" s="21" t="s">
+        <v>55</v>
+      </c>
+      <c r="E177" s="39" t="s">
+        <v>213</v>
+      </c>
+      <c r="F177" s="8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="178">
+      <c r="A178" s="40" t="s">
+        <v>70</v>
+      </c>
+      <c r="B178" s="41">
+        <v>7.0</v>
+      </c>
+      <c r="C178" s="42" t="s">
+        <v>197</v>
+      </c>
+      <c r="D178" s="21" t="s">
+        <v>58</v>
+      </c>
+      <c r="E178" s="39" t="s">
+        <v>214</v>
+      </c>
+      <c r="F178" s="8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="179">
+      <c r="A179" s="40" t="s">
+        <v>70</v>
+      </c>
+      <c r="B179" s="41">
+        <v>7.0</v>
+      </c>
+      <c r="C179" s="42" t="s">
+        <v>197</v>
+      </c>
+      <c r="D179" s="21" t="s">
+        <v>61</v>
+      </c>
+      <c r="E179" s="39" t="s">
+        <v>215</v>
+      </c>
+      <c r="F179" s="8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="180">
+      <c r="A180" s="40" t="s">
+        <v>70</v>
+      </c>
+      <c r="B180" s="41">
+        <v>7.0</v>
+      </c>
+      <c r="C180" s="42" t="s">
+        <v>197</v>
+      </c>
+      <c r="D180" s="21" t="s">
+        <v>64</v>
+      </c>
+      <c r="E180" s="39" t="s">
+        <v>216</v>
+      </c>
+      <c r="F180" s="8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="181">
+      <c r="A181" s="40" t="s">
+        <v>70</v>
+      </c>
+      <c r="B181" s="41">
+        <v>7.0</v>
+      </c>
+      <c r="C181" s="42" t="s">
+        <v>197</v>
+      </c>
+      <c r="D181" s="21" t="s">
+        <v>67</v>
+      </c>
+      <c r="E181" s="39" t="s">
+        <v>217</v>
+      </c>
+      <c r="F181" s="8" t="s">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>